<commit_message>
Started with the Creation of the Level Select Screen
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/Guppen-Planung.xlsx
+++ b/01_ProjectPlanning/Guppen-Planung.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>Task</t>
   </si>
@@ -146,12 +146,24 @@
   </si>
   <si>
     <t>Bugfixing siehe Bugs.xlsx Didn't fixed all Bugs</t>
+  </si>
+  <si>
+    <t>Sprite für Schweinchenhexe</t>
+  </si>
+  <si>
+    <t>Steffi</t>
+  </si>
+  <si>
+    <t>Hexenhütte</t>
+  </si>
+  <si>
+    <t>Inside of the Hut of the adventurer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -294,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -320,9 +332,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -338,6 +347,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -386,7 +405,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -672,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,30 +738,30 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="22">
-        <v>6</v>
-      </c>
-      <c r="C2" s="22">
+      <c r="B2" s="21">
+        <v>6</v>
+      </c>
+      <c r="C2" s="21">
         <v>2.5</v>
       </c>
-      <c r="D2" s="22">
-        <v>1</v>
-      </c>
-      <c r="E2" s="22">
+      <c r="D2" s="21">
+        <v>1</v>
+      </c>
+      <c r="E2" s="21">
         <f>C2-D2</f>
         <v>1.5</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="22">
         <f t="shared" ref="G2" si="0">1-E2/C2</f>
         <v>0.4</v>
       </c>
-      <c r="H2" s="24" t="str">
+      <c r="H2" s="23" t="str">
         <f>IF(G2=100%,"✔","X")</f>
         <v>X</v>
       </c>
@@ -751,64 +770,68 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="A3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="24">
+        <v>6</v>
+      </c>
+      <c r="C3" s="21">
         <v>5.5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="21">
         <v>2</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="21">
         <f>C3-D3</f>
         <v>3.5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G26" si="1">1-E3/C3</f>
+      <c r="G3" s="22">
+        <f t="shared" ref="G3:G49" si="1">1-E3/C3</f>
         <v>0.36363636363636365</v>
       </c>
-      <c r="H3" s="12" t="str">
+      <c r="H3" s="23" t="str">
         <f>IF(G3=100%,"✔","X")</f>
         <v>X</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" s="24">
+        <v>3</v>
+      </c>
+      <c r="C4" s="21">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="D4" s="21">
+        <v>0</v>
+      </c>
+      <c r="E4" s="21">
         <f t="shared" ref="E4:E8" si="2">C4-D4</f>
         <v>2</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H4" s="12" t="str">
-        <f t="shared" ref="H4:H26" si="3">IF(G4=100%,"✔","X")</f>
+      <c r="G4" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="23" t="str">
+        <f t="shared" ref="H4:H49" si="3">IF(G4=100%,"✔","X")</f>
         <v>X</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -944,7 +967,7 @@
         <v>1.5</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" ref="E9:E26" si="4">C9-D9</f>
+        <f t="shared" ref="E9:E49" si="4">C9-D9</f>
         <v>0</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1025,62 +1048,62 @@
       <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="18">
-        <v>3</v>
-      </c>
-      <c r="C12" s="17">
-        <v>3</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="B12" s="17">
+        <v>3</v>
+      </c>
+      <c r="C12" s="16">
+        <v>3</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="20" t="str">
+      <c r="G12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="19" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="4">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="B13" s="24">
+        <v>6</v>
+      </c>
+      <c r="C13" s="21">
+        <v>6</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="15" t="str">
+      <c r="G13" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="29" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="I13" s="16"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1443,24 +1466,512 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H26" s="12" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="F26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H26" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>✔</v>
       </c>
       <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="C27" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="D27" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="E27" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H27" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>✔</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="25">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>X</v>
+      </c>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H34" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H36" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H37" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H38" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H39" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H41" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H42" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H43" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H44" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H45" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H46" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H47" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H48" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H49" s="28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I49" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented VS Studio Integration with Unity, Updated Story
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/Guppen-Planung.xlsx
+++ b/01_ProjectPlanning/Guppen-Planung.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>Inside of the Hut of the adventurer</t>
+  </si>
+  <si>
+    <t>Golem Sprite</t>
+  </si>
+  <si>
+    <t>End Sequence for first Level</t>
+  </si>
+  <si>
+    <t>Rotation of the player by Mouse Movement Fix</t>
+  </si>
+  <si>
+    <t>SquirelWurf Skript</t>
   </si>
 </sst>
 </file>
@@ -694,7 +706,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,34 +1118,34 @@
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="4">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="B14" s="24">
+        <v>3</v>
+      </c>
+      <c r="C14" s="21">
+        <v>3</v>
+      </c>
+      <c r="D14" s="21">
+        <v>3</v>
+      </c>
+      <c r="E14" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H14" s="12" t="str">
+      <c r="G14" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H14" s="23" t="str">
         <f t="shared" si="3"/>
         <v>✔</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1238,22 +1250,22 @@
         <v>9</v>
       </c>
       <c r="D18" s="4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="1"/>
-        <v>0.44444444444444442</v>
+        <v>1</v>
       </c>
       <c r="H18" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -1297,21 +1309,23 @@
       <c r="C20" s="1">
         <v>10</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1">
+        <v>10</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -1387,21 +1401,23 @@
       <c r="C23" s="1">
         <v>3</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I23" s="1"/>
     </row>
@@ -1533,19 +1549,21 @@
         <v>2</v>
       </c>
       <c r="C28" s="1">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
       <c r="E28" s="25">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G28" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H28" s="28" t="str">
         <f t="shared" si="3"/>
@@ -1554,82 +1572,120 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2.5</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="25">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H29" s="28" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>2.5</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>X</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="1">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
       <c r="E30" s="25">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H30" s="28" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="27">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="H30" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>X</v>
       </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
       <c r="E31" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H31" s="28" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="F31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H31" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>✔</v>
       </c>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="1">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
       <c r="E32" s="25">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H32" s="28" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="27">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="H32" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>X</v>
       </c>
       <c r="I32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added Rocking Animation for Adventurer who is sitting in the Hut
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/Guppen-Planung.xlsx
+++ b/01_ProjectPlanning/Guppen-Planung.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t>Task</t>
   </si>
@@ -157,12 +157,6 @@
     <t>Hexenhütte</t>
   </si>
   <si>
-    <t>Inside of the Hut of the adventurer</t>
-  </si>
-  <si>
-    <t>Golem Sprite</t>
-  </si>
-  <si>
     <t>End Sequence for first Level</t>
   </si>
   <si>
@@ -170,6 +164,27 @@
   </si>
   <si>
     <t>SquirelWurf Skript</t>
+  </si>
+  <si>
+    <t>Implement General Boss Healthbar</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Villager Sprites (20)</t>
+  </si>
+  <si>
+    <t>Iphi Sprite + Animation</t>
+  </si>
+  <si>
+    <t>Flicker Script for Hut of Adventurer</t>
+  </si>
+  <si>
+    <t>The square should be dynamicly arranged around the artifacts which are used to select the level</t>
+  </si>
+  <si>
+    <t>Basic Level Selection for Inside of Hut + Implement dynamic Square for Level Selection</t>
   </si>
 </sst>
 </file>
@@ -706,7 +721,8 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,211 +1559,243 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="C28" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E28" s="25">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f>C28-D28</f>
+        <v>3.5</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="G28" s="27">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
+        <f>1-E28/C28</f>
+        <v>0.41666666666666663</v>
       </c>
       <c r="H28" s="28" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(G28=100%,"✔","X")</f>
         <v>X</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="D29" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
       <c r="E29" s="25">
-        <f t="shared" si="4"/>
-        <v>2.5</v>
+        <f>C29-D29</f>
+        <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="G29" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>1-E29/C29</f>
+        <v>0.75</v>
       </c>
       <c r="H29" s="28" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(G29=100%,"✔","X")</f>
         <v>X</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C30" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E30" s="25">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>C30-D30</f>
+        <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G30" s="27">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <f>1-E30/C30</f>
+        <v>1</v>
       </c>
       <c r="H30" s="28" t="str">
-        <f t="shared" si="3"/>
-        <v>X</v>
+        <f>IF(G30=100%,"✔","X")</f>
+        <v>✔</v>
       </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E31" s="25">
-        <f t="shared" si="4"/>
+        <f>C31-D31</f>
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G31" s="27">
-        <f t="shared" si="1"/>
+        <f>1-E31/C31</f>
         <v>1</v>
       </c>
       <c r="H31" s="28" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(G31=100%,"✔","X")</f>
         <v>✔</v>
       </c>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="1">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>3</v>
+      </c>
+      <c r="E32" s="25">
+        <f>C32-D32</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="27">
+        <v>0</v>
+      </c>
+      <c r="H32" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="1">
-        <v>3</v>
-      </c>
-      <c r="C32" s="1">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="1">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1">
+        <v>4</v>
+      </c>
+      <c r="E33" s="25">
+        <f>C33-D33</f>
         <v>2</v>
       </c>
-      <c r="E32" s="25">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G32" s="27">
-        <f t="shared" si="1"/>
+      <c r="F33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="27">
+        <f>1-E33/C33</f>
         <v>0.66666666666666674</v>
       </c>
-      <c r="H32" s="28" t="str">
-        <f t="shared" si="3"/>
+      <c r="H33" s="28" t="str">
+        <f>IF(G33=100%,"✔","X")</f>
         <v>X</v>
       </c>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H33" s="28" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2</v>
+      </c>
       <c r="E34" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H34" s="28" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <f>C34-D34</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="27">
+        <f>1-E34/C34</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="28" t="str">
+        <f>IF(G34=100%,"✔","X")</f>
+        <v>✔</v>
       </c>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H35" s="28" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <f>C35-D35</f>
+        <v>3</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="1">
+        <f>1-E35/C35</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="28" t="str">
+        <f>IF(G35=100%,"✔","X")</f>
+        <v>X</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
@@ -1764,10 +1812,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H36" s="28" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I36" s="1"/>
+        <f t="shared" ref="H36:H49" si="5">IF(G36=100%,"✔","X")</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
@@ -1784,7 +1831,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H37" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I37" s="1"/>
@@ -1804,7 +1851,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H38" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I38" s="1"/>
@@ -1824,7 +1871,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H39" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I39" s="1"/>
@@ -1844,7 +1891,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H40" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I40" s="1"/>
@@ -1864,7 +1911,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H41" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I41" s="1"/>
@@ -1884,7 +1931,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H42" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I42" s="1"/>
@@ -1904,7 +1951,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H43" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I43" s="1"/>
@@ -1924,7 +1971,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H44" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I44" s="1"/>
@@ -1944,7 +1991,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H45" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I45" s="1"/>
@@ -1964,7 +2011,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H46" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I46" s="1"/>
@@ -1984,7 +2031,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H47" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I47" s="1"/>
@@ -2004,7 +2051,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H48" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I48" s="1"/>
@@ -2024,7 +2071,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H49" s="28" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I49" s="1"/>

</xml_diff>

<commit_message>
Release 02 of "The Adventures of an Adventurer" + Release and Planing Docs
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/Guppen-Planung.xlsx
+++ b/01_ProjectPlanning/Guppen-Planung.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
   <si>
     <t>Task</t>
   </si>
@@ -239,12 +239,24 @@
   </si>
   <si>
     <t>Health UI for Enemies</t>
+  </si>
+  <si>
+    <t>Porky(enemy) implementation in game</t>
+  </si>
+  <si>
+    <t>Bat enemy implementation</t>
+  </si>
+  <si>
+    <t>Implement first level (Basic Colliders, "Decoration")</t>
+  </si>
+  <si>
+    <t>Cedric, Sascha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -505,7 +517,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -580,6 +592,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -615,6 +644,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -794,24 +840,24 @@
   <dimension ref="A1:K232"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="93" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="77.36328125" customWidth="1"/>
-    <col min="2" max="3" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.33203125" customWidth="1"/>
+    <col min="2" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6328125" customWidth="1"/>
-    <col min="11" max="11" width="144.6328125" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="144.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -846,7 +892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>16</v>
       </c>
@@ -880,7 +926,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
@@ -914,7 +960,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>5</v>
       </c>
@@ -948,7 +994,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -980,7 +1026,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1014,7 +1060,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1048,7 +1094,7 @@
       <c r="J7" s="12"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -1082,7 +1128,7 @@
       <c r="J8" s="30"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1118,7 +1164,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>21</v>
       </c>
@@ -1152,7 +1198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>23</v>
       </c>
@@ -1186,7 +1232,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
@@ -1218,7 +1264,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>26</v>
       </c>
@@ -1248,7 +1294,7 @@
       <c r="J13" s="29"/>
       <c r="K13" s="15"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>29</v>
       </c>
@@ -1280,7 +1326,7 @@
       <c r="J14" s="31"/>
       <c r="K14" s="16"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1290,21 +1336,23 @@
       <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I15" s="12">
         <v>34</v>
@@ -1314,7 +1362,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>30</v>
       </c>
@@ -1348,7 +1396,7 @@
       <c r="J16" s="14"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
@@ -1384,7 +1432,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1418,7 +1466,7 @@
       <c r="J18" s="12"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1450,7 +1498,7 @@
       <c r="J19" s="12"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
@@ -1484,7 +1532,7 @@
       <c r="J20" s="12"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1518,7 +1566,7 @@
       <c r="J21" s="12"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -1552,7 +1600,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
@@ -1586,7 +1634,7 @@
       <c r="J23" s="12"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -1620,7 +1668,7 @@
       <c r="J24" s="12"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
@@ -1654,7 +1702,7 @@
       <c r="J25" s="12"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
@@ -1688,7 +1736,7 @@
       <c r="J26" s="12"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>44</v>
       </c>
@@ -1722,7 +1770,7 @@
       <c r="J27" s="28"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1756,7 +1804,7 @@
       <c r="J28" s="28"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -1790,7 +1838,7 @@
       <c r="J29" s="28"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
@@ -1824,7 +1872,7 @@
       <c r="J30" s="28"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -1858,7 +1906,7 @@
       <c r="J31" s="28"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
@@ -1892,7 +1940,7 @@
       <c r="J32" s="28"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
@@ -1926,7 +1974,7 @@
       <c r="J33" s="28"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
@@ -1960,7 +2008,7 @@
       <c r="J34" s="28"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>50</v>
       </c>
@@ -1971,22 +2019,22 @@
         <v>5</v>
       </c>
       <c r="D35" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="H35" s="28" t="str">
         <f>IF(G35=100%,"✔","X")</f>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I35" s="28">
         <v>4</v>
@@ -1996,7 +2044,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>52</v>
       </c>
@@ -2029,7 +2077,7 @@
       </c>
       <c r="J36" s="28"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>51</v>
       </c>
@@ -2063,7 +2111,7 @@
       <c r="J37" s="28"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>55</v>
       </c>
@@ -2097,7 +2145,7 @@
       <c r="J38" s="28"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>60</v>
       </c>
@@ -2131,7 +2179,7 @@
       <c r="J39" s="28"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
@@ -2165,7 +2213,7 @@
       <c r="J40" s="28"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>62</v>
       </c>
@@ -2199,7 +2247,7 @@
       <c r="J41" s="28"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
@@ -2233,7 +2281,7 @@
       <c r="J42" s="28"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>64</v>
       </c>
@@ -2267,7 +2315,7 @@
       <c r="J43" s="28"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -2301,7 +2349,7 @@
       <c r="J44" s="28"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>66</v>
       </c>
@@ -2335,7 +2383,7 @@
       <c r="J45" s="28"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>67</v>
       </c>
@@ -2369,7 +2417,7 @@
       <c r="J46" s="28"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>68</v>
       </c>
@@ -2403,7 +2451,7 @@
       <c r="J47" s="28"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>69</v>
       </c>
@@ -2437,7 +2485,7 @@
       <c r="J48" s="28"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>70</v>
       </c>
@@ -2471,7 +2519,7 @@
       <c r="J49" s="28"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="25" t="s">
         <v>71</v>
       </c>
@@ -2482,22 +2530,22 @@
         <v>10</v>
       </c>
       <c r="D50" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E50" s="1">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G50" s="3">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H50" s="12" t="str">
         <f t="shared" si="7"/>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I50" s="12">
         <v>42</v>
@@ -2505,7 +2553,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="25" t="s">
         <v>72</v>
       </c>
@@ -2513,23 +2561,25 @@
         <v>3</v>
       </c>
       <c r="C51" s="1">
-        <v>3</v>
-      </c>
-      <c r="D51" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D51" s="1">
+        <v>4</v>
+      </c>
       <c r="E51" s="1">
         <f>C51-D51</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G51" s="3">
         <f t="shared" ref="G51" si="8">1-E51/C51</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" s="12" t="str">
         <f t="shared" ref="H51" si="9">IF(G51=100%,"✔","X")</f>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I51" s="12">
         <v>47</v>
@@ -2537,7 +2587,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="25" t="s">
         <v>73</v>
       </c>
@@ -2547,21 +2597,23 @@
       <c r="C52" s="1">
         <v>6</v>
       </c>
-      <c r="D52" s="1"/>
+      <c r="D52" s="1">
+        <v>6</v>
+      </c>
       <c r="E52" s="1">
         <f t="shared" ref="E52:E115" si="10">C52-D52</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G52" s="3">
         <f t="shared" ref="G52:G115" si="11">1-E52/C52</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" s="12" t="str">
         <f t="shared" ref="H52:H115" si="12">IF(G52=100%,"✔","X")</f>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I52" s="12">
         <v>30</v>
@@ -2569,73 +2621,107 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A53" s="25"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="1">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1">
+        <v>5</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2</v>
+      </c>
       <c r="E53" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="3" t="e">
+        <v>3</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="3">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H53" s="12" t="e">
+        <v>0.4</v>
+      </c>
+      <c r="H53" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I53" s="12"/>
+        <v>X</v>
+      </c>
+      <c r="I53" s="12">
+        <v>13</v>
+      </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A54" s="25"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="1">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1">
+        <v>4</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
       <c r="E54" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="3" t="e">
+        <v>4</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="3">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H54" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="H54" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I54" s="12"/>
+        <v>X</v>
+      </c>
+      <c r="I54" s="12">
+        <v>13</v>
+      </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55" s="25"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="1">
+        <v>3</v>
+      </c>
+      <c r="C55" s="1">
+        <v>3</v>
+      </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="3" t="e">
+        <v>3</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G55" s="3">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H55" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="H55" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I55" s="12"/>
+        <v>X</v>
+      </c>
+      <c r="I55" s="12">
+        <v>13</v>
+      </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="25"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2657,7 +2743,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="25"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2679,7 +2765,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="25"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2701,7 +2787,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="25"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2723,7 +2809,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="25"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2745,7 +2831,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="25"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2767,7 +2853,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="25"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2789,7 +2875,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="25"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2811,7 +2897,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="25"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2833,7 +2919,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="25"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2855,7 +2941,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="25"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2877,7 +2963,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="25"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2899,7 +2985,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="25"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2921,7 +3007,7 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="25"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2943,7 +3029,7 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="25"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2965,7 +3051,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="25"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2987,7 +3073,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="25"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3009,7 +3095,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="25"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3031,7 +3117,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="25"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3053,7 +3139,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="25"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3075,7 +3161,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="25"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3097,7 +3183,7 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="25"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3119,7 +3205,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="25"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3141,7 +3227,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="25"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3163,7 +3249,7 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="25"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3185,7 +3271,7 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="25"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3207,7 +3293,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="25"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3229,7 +3315,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="25"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3251,7 +3337,7 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="25"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3273,7 +3359,7 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="25"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3295,7 +3381,7 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="25"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3317,7 +3403,7 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="25"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3339,7 +3425,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="25"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3361,7 +3447,7 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="25"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3383,7 +3469,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="25"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3405,7 +3491,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="25"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3427,7 +3513,7 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="25"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3449,7 +3535,7 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="25"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3471,7 +3557,7 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="25"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3493,7 +3579,7 @@
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="25"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3515,7 +3601,7 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="25"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3537,7 +3623,7 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="25"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3559,7 +3645,7 @@
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="25"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3581,7 +3667,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="25"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3603,7 +3689,7 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="25"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3625,7 +3711,7 @@
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="25"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3647,7 +3733,7 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="25"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3669,7 +3755,7 @@
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="25"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3691,7 +3777,7 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="25"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3713,7 +3799,7 @@
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="25"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3735,7 +3821,7 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="25"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3757,7 +3843,7 @@
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="25"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3779,7 +3865,7 @@
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="25"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3801,7 +3887,7 @@
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="25"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3823,7 +3909,7 @@
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="25"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3845,7 +3931,7 @@
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="25"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3867,7 +3953,7 @@
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="25"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3889,7 +3975,7 @@
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="25"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3911,7 +3997,7 @@
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="25"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3933,7 +4019,7 @@
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="25"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3955,7 +4041,7 @@
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="25"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3977,7 +4063,7 @@
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="25"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3999,7 +4085,7 @@
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="25"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -4021,7 +4107,7 @@
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="25"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -4043,7 +4129,7 @@
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="25"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -4065,7 +4151,7 @@
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="25"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -4087,7 +4173,7 @@
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="25"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -4109,7 +4195,7 @@
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="25"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -4131,7 +4217,7 @@
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="25"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -4153,7 +4239,7 @@
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="25"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -4175,7 +4261,7 @@
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="25"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -4197,7 +4283,7 @@
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="25"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -4219,7 +4305,7 @@
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="25"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -4241,7 +4327,7 @@
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="25"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -4263,7 +4349,7 @@
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="25"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -4285,7 +4371,7 @@
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="25"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -4307,7 +4393,7 @@
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="25"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -4329,7 +4415,7 @@
       <c r="J132" s="1"/>
       <c r="K132" s="1"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="25"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -4351,7 +4437,7 @@
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="25"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -4373,7 +4459,7 @@
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="25"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -4395,7 +4481,7 @@
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" s="25"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -4417,7 +4503,7 @@
       <c r="J136" s="1"/>
       <c r="K136" s="1"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" s="25"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -4439,7 +4525,7 @@
       <c r="J137" s="1"/>
       <c r="K137" s="1"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="25"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -4461,7 +4547,7 @@
       <c r="J138" s="1"/>
       <c r="K138" s="1"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="25"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -4483,7 +4569,7 @@
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" s="25"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -4505,7 +4591,7 @@
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" s="25"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -4527,7 +4613,7 @@
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" s="25"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -4549,7 +4635,7 @@
       <c r="J142" s="1"/>
       <c r="K142" s="1"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" s="25"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -4571,7 +4657,7 @@
       <c r="J143" s="1"/>
       <c r="K143" s="1"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" s="25"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -4593,7 +4679,7 @@
       <c r="J144" s="1"/>
       <c r="K144" s="1"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" s="25"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -4615,7 +4701,7 @@
       <c r="J145" s="1"/>
       <c r="K145" s="1"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="25"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -4637,7 +4723,7 @@
       <c r="J146" s="1"/>
       <c r="K146" s="1"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="25"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -4659,7 +4745,7 @@
       <c r="J147" s="1"/>
       <c r="K147" s="1"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="25"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -4681,7 +4767,7 @@
       <c r="J148" s="1"/>
       <c r="K148" s="1"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" s="25"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -4703,7 +4789,7 @@
       <c r="J149" s="1"/>
       <c r="K149" s="1"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" s="25"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -4725,7 +4811,7 @@
       <c r="J150" s="1"/>
       <c r="K150" s="1"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" s="25"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4747,7 +4833,7 @@
       <c r="J151" s="1"/>
       <c r="K151" s="1"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="25"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -4769,7 +4855,7 @@
       <c r="J152" s="1"/>
       <c r="K152" s="1"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="25"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4791,7 +4877,7 @@
       <c r="J153" s="1"/>
       <c r="K153" s="1"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" s="25"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4813,7 +4899,7 @@
       <c r="J154" s="1"/>
       <c r="K154" s="1"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" s="25"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4835,7 +4921,7 @@
       <c r="J155" s="1"/>
       <c r="K155" s="1"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" s="25"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4857,7 +4943,7 @@
       <c r="J156" s="1"/>
       <c r="K156" s="1"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" s="25"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4879,7 +4965,7 @@
       <c r="J157" s="1"/>
       <c r="K157" s="1"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" s="25"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4901,7 +4987,7 @@
       <c r="J158" s="1"/>
       <c r="K158" s="1"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" s="25"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4923,7 +5009,7 @@
       <c r="J159" s="1"/>
       <c r="K159" s="1"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" s="25"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4945,7 +5031,7 @@
       <c r="J160" s="1"/>
       <c r="K160" s="1"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" s="25"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4967,7 +5053,7 @@
       <c r="J161" s="1"/>
       <c r="K161" s="1"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" s="25"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4989,7 +5075,7 @@
       <c r="J162" s="1"/>
       <c r="K162" s="1"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" s="25"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -5011,7 +5097,7 @@
       <c r="J163" s="1"/>
       <c r="K163" s="1"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" s="25"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -5033,7 +5119,7 @@
       <c r="J164" s="1"/>
       <c r="K164" s="1"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" s="25"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -5055,7 +5141,7 @@
       <c r="J165" s="1"/>
       <c r="K165" s="1"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" s="25"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -5077,7 +5163,7 @@
       <c r="J166" s="1"/>
       <c r="K166" s="1"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" s="25"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -5099,7 +5185,7 @@
       <c r="J167" s="1"/>
       <c r="K167" s="1"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" s="25"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -5121,7 +5207,7 @@
       <c r="J168" s="1"/>
       <c r="K168" s="1"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" s="25"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -5143,7 +5229,7 @@
       <c r="J169" s="1"/>
       <c r="K169" s="1"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" s="25"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -5165,7 +5251,7 @@
       <c r="J170" s="1"/>
       <c r="K170" s="1"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" s="25"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -5187,7 +5273,7 @@
       <c r="J171" s="1"/>
       <c r="K171" s="1"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" s="25"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -5209,7 +5295,7 @@
       <c r="J172" s="1"/>
       <c r="K172" s="1"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" s="25"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -5231,7 +5317,7 @@
       <c r="J173" s="1"/>
       <c r="K173" s="1"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" s="25"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -5253,7 +5339,7 @@
       <c r="J174" s="1"/>
       <c r="K174" s="1"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175" s="25"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -5275,7 +5361,7 @@
       <c r="J175" s="1"/>
       <c r="K175" s="1"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176" s="25"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -5297,7 +5383,7 @@
       <c r="J176" s="1"/>
       <c r="K176" s="1"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177" s="25"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -5319,7 +5405,7 @@
       <c r="J177" s="1"/>
       <c r="K177" s="1"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178" s="25"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -5341,7 +5427,7 @@
       <c r="J178" s="1"/>
       <c r="K178" s="1"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179" s="25"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -5363,7 +5449,7 @@
       <c r="J179" s="1"/>
       <c r="K179" s="1"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180" s="25"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -5385,7 +5471,7 @@
       <c r="J180" s="1"/>
       <c r="K180" s="1"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181" s="25"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -5407,7 +5493,7 @@
       <c r="J181" s="1"/>
       <c r="K181" s="1"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182" s="25"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -5429,7 +5515,7 @@
       <c r="J182" s="1"/>
       <c r="K182" s="1"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183" s="25"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -5451,7 +5537,7 @@
       <c r="J183" s="1"/>
       <c r="K183" s="1"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184" s="25"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -5473,7 +5559,7 @@
       <c r="J184" s="1"/>
       <c r="K184" s="1"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185" s="25"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -5495,7 +5581,7 @@
       <c r="J185" s="1"/>
       <c r="K185" s="1"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186" s="25"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -5517,7 +5603,7 @@
       <c r="J186" s="1"/>
       <c r="K186" s="1"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187" s="25"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -5539,7 +5625,7 @@
       <c r="J187" s="1"/>
       <c r="K187" s="1"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188" s="25"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -5561,7 +5647,7 @@
       <c r="J188" s="1"/>
       <c r="K188" s="1"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189" s="25"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -5583,7 +5669,7 @@
       <c r="J189" s="1"/>
       <c r="K189" s="1"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190" s="25"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -5605,7 +5691,7 @@
       <c r="J190" s="1"/>
       <c r="K190" s="1"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191" s="25"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -5627,7 +5713,7 @@
       <c r="J191" s="1"/>
       <c r="K191" s="1"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192" s="25"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -5649,7 +5735,7 @@
       <c r="J192" s="1"/>
       <c r="K192" s="1"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193" s="25"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -5671,7 +5757,7 @@
       <c r="J193" s="1"/>
       <c r="K193" s="1"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194" s="25"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -5693,7 +5779,7 @@
       <c r="J194" s="1"/>
       <c r="K194" s="1"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195" s="25"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -5715,7 +5801,7 @@
       <c r="J195" s="1"/>
       <c r="K195" s="1"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A196" s="25"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -5737,7 +5823,7 @@
       <c r="J196" s="1"/>
       <c r="K196" s="1"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197" s="25"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -5759,7 +5845,7 @@
       <c r="J197" s="1"/>
       <c r="K197" s="1"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A198" s="25"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -5781,7 +5867,7 @@
       <c r="J198" s="1"/>
       <c r="K198" s="1"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199" s="25"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -5803,7 +5889,7 @@
       <c r="J199" s="1"/>
       <c r="K199" s="1"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A200" s="25"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -5825,7 +5911,7 @@
       <c r="J200" s="1"/>
       <c r="K200" s="1"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A201" s="25"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -5847,7 +5933,7 @@
       <c r="J201" s="1"/>
       <c r="K201" s="1"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A202" s="25"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -5869,7 +5955,7 @@
       <c r="J202" s="1"/>
       <c r="K202" s="1"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A203" s="25"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -5891,7 +5977,7 @@
       <c r="J203" s="1"/>
       <c r="K203" s="1"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A204" s="25"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -5913,7 +5999,7 @@
       <c r="J204" s="1"/>
       <c r="K204" s="1"/>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A205" s="25"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -5935,7 +6021,7 @@
       <c r="J205" s="1"/>
       <c r="K205" s="1"/>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A206" s="25"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -5957,7 +6043,7 @@
       <c r="J206" s="1"/>
       <c r="K206" s="1"/>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A207" s="25"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -5979,7 +6065,7 @@
       <c r="J207" s="1"/>
       <c r="K207" s="1"/>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A208" s="25"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -6001,7 +6087,7 @@
       <c r="J208" s="1"/>
       <c r="K208" s="1"/>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A209" s="25"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -6023,7 +6109,7 @@
       <c r="J209" s="1"/>
       <c r="K209" s="1"/>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A210" s="25"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -6045,7 +6131,7 @@
       <c r="J210" s="1"/>
       <c r="K210" s="1"/>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A211" s="25"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -6067,7 +6153,7 @@
       <c r="J211" s="1"/>
       <c r="K211" s="1"/>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A212" s="25"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -6089,7 +6175,7 @@
       <c r="J212" s="1"/>
       <c r="K212" s="1"/>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A213" s="25"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -6111,7 +6197,7 @@
       <c r="J213" s="1"/>
       <c r="K213" s="1"/>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A214" s="25"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -6133,7 +6219,7 @@
       <c r="J214" s="1"/>
       <c r="K214" s="1"/>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A215" s="25"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -6155,7 +6241,7 @@
       <c r="J215" s="1"/>
       <c r="K215" s="1"/>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A216" s="25"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -6177,7 +6263,7 @@
       <c r="J216" s="1"/>
       <c r="K216" s="1"/>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A217" s="25"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -6199,7 +6285,7 @@
       <c r="J217" s="1"/>
       <c r="K217" s="1"/>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A218" s="25"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -6221,7 +6307,7 @@
       <c r="J218" s="1"/>
       <c r="K218" s="1"/>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A219" s="25"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -6243,7 +6329,7 @@
       <c r="J219" s="1"/>
       <c r="K219" s="1"/>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A220" s="25"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -6265,7 +6351,7 @@
       <c r="J220" s="1"/>
       <c r="K220" s="1"/>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A221" s="25"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -6287,7 +6373,7 @@
       <c r="J221" s="1"/>
       <c r="K221" s="1"/>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A222" s="25"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -6309,7 +6395,7 @@
       <c r="J222" s="1"/>
       <c r="K222" s="1"/>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A223" s="25"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -6331,7 +6417,7 @@
       <c r="J223" s="1"/>
       <c r="K223" s="1"/>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A224" s="25"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -6353,7 +6439,7 @@
       <c r="J224" s="1"/>
       <c r="K224" s="1"/>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A225" s="25"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -6375,7 +6461,7 @@
       <c r="J225" s="1"/>
       <c r="K225" s="1"/>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A226" s="25"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -6397,7 +6483,7 @@
       <c r="J226" s="1"/>
       <c r="K226" s="1"/>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A227" s="25"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -6419,7 +6505,7 @@
       <c r="J227" s="1"/>
       <c r="K227" s="1"/>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A228" s="25"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -6441,7 +6527,7 @@
       <c r="J228" s="1"/>
       <c r="K228" s="1"/>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A229" s="25"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -6463,7 +6549,7 @@
       <c r="J229" s="1"/>
       <c r="K229" s="1"/>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A230" s="25"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -6485,7 +6571,7 @@
       <c r="J230" s="1"/>
       <c r="K230" s="1"/>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A231" s="25"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -6507,7 +6593,7 @@
       <c r="J231" s="1"/>
       <c r="K231" s="1"/>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A232" s="25"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>

</xml_diff>